<commit_message>
intermediate for loading data
</commit_message>
<xml_diff>
--- a/data_tables.xlsx
+++ b/data_tables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Venkata Sai\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratiksaxena/projects/gameopedia/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E7FB09-8609-BB4B-B910-9217BE83D457}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="820" yWindow="500" windowWidth="27980" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Games" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="102">
   <si>
     <t>Game Name</t>
   </si>
@@ -247,18 +248,9 @@
     <t>https://i.imgur.com/ZnTnDcG.png</t>
   </si>
   <si>
-    <t>User</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
-    <t>PREFERENCES</t>
-  </si>
-  <si>
-    <t>Game Name (key)</t>
-  </si>
-  <si>
     <t>Game Category: Genres</t>
   </si>
   <si>
@@ -322,9 +314,6 @@
     <t>Shooting, Strategy</t>
   </si>
   <si>
-    <t>No Result</t>
-  </si>
-  <si>
     <t>Roberto</t>
   </si>
   <si>
@@ -341,12 +330,15 @@
   </si>
   <si>
     <t>Violence</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -388,27 +380,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB6D7A8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF666666"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -483,93 +463,6 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
       <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
@@ -581,7 +474,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -610,40 +503,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -926,24 +786,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="1" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -963,7 +823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="2" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -983,7 +843,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="3" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
@@ -1003,7 +863,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="4" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
@@ -1023,7 +883,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="5" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A5" s="7" t="s">
         <v>23</v>
       </c>
@@ -1043,7 +903,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="6" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1063,7 +923,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="7" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A7" s="7" t="s">
         <v>29</v>
       </c>
@@ -1083,7 +943,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="8" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A8" s="7" t="s">
         <v>32</v>
       </c>
@@ -1103,7 +963,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="9" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
@@ -1123,7 +983,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="10" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A10" s="7" t="s">
         <v>37</v>
       </c>
@@ -1143,7 +1003,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="11" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -1163,7 +1023,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="12" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A12" s="7" t="s">
         <v>42</v>
       </c>
@@ -1183,7 +1043,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="13" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A13" s="7" t="s">
         <v>45</v>
       </c>
@@ -1203,7 +1063,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="14" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A14" s="7" t="s">
         <v>47</v>
       </c>
@@ -1223,7 +1083,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="15" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A15" s="7" t="s">
         <v>49</v>
       </c>
@@ -1243,7 +1103,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="16" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -1263,7 +1123,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="17" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -1283,7 +1143,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="18" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A18" s="7" t="s">
         <v>55</v>
       </c>
@@ -1303,7 +1163,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="19" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A19" s="7" t="s">
         <v>57</v>
       </c>
@@ -1323,7 +1183,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="20" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A20" s="7" t="s">
         <v>59</v>
       </c>
@@ -1343,7 +1203,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="21" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A21" s="7" t="s">
         <v>61</v>
       </c>
@@ -1363,7 +1223,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="22" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A22" s="7" t="s">
         <v>63</v>
       </c>
@@ -1383,7 +1243,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="23" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A23" s="7" t="s">
         <v>65</v>
       </c>
@@ -1403,7 +1263,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="24" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A24" s="7" t="s">
         <v>67</v>
       </c>
@@ -1423,7 +1283,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="25" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A25" s="7" t="s">
         <v>69</v>
       </c>
@@ -1443,7 +1303,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="26" spans="1:6" ht="20" customHeight="1" thickBot="1">
       <c r="A26" s="7" t="s">
         <v>71</v>
       </c>
@@ -1465,31 +1325,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-    <hyperlink ref="B12" r:id="rId11"/>
-    <hyperlink ref="B13" r:id="rId12"/>
-    <hyperlink ref="B14" r:id="rId13"/>
-    <hyperlink ref="B15" r:id="rId14"/>
-    <hyperlink ref="B16" r:id="rId15"/>
-    <hyperlink ref="B17" r:id="rId16"/>
-    <hyperlink ref="B18" r:id="rId17"/>
-    <hyperlink ref="B19" r:id="rId18"/>
-    <hyperlink ref="B20" r:id="rId19"/>
-    <hyperlink ref="B21" r:id="rId20"/>
-    <hyperlink ref="B22" r:id="rId21"/>
-    <hyperlink ref="B23" r:id="rId22"/>
-    <hyperlink ref="B24" r:id="rId23"/>
-    <hyperlink ref="B25" r:id="rId24"/>
-    <hyperlink ref="B26" r:id="rId25"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId26"/>
@@ -1497,519 +1357,211 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:5" ht="30" thickBot="1">
+      <c r="A1" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="E1" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" thickBot="1">
+      <c r="A2" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="20" t="s">
+      <c r="B2" s="9">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="52.5" thickBot="1">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="21"/>
-    </row>
-    <row r="3" spans="1:6" ht="39.75" thickBot="1">
+      <c r="E2" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16" thickBot="1">
       <c r="A3" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B3" s="9">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>80</v>
+        <v>21</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="27" thickBot="1">
-      <c r="A4" s="7"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="10" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="16" thickBot="1">
+      <c r="A4" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="9">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16" thickBot="1">
+      <c r="A5" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="9">
+        <v>17</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16" thickBot="1">
+      <c r="A6" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="9">
+        <v>32</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16" thickBot="1">
+      <c r="A7" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="9">
+        <v>26</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16" thickBot="1">
+      <c r="A8" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="9">
+        <v>12</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16" thickBot="1">
+      <c r="A9" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="9">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="27" thickBot="1">
-      <c r="A5" s="7"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="1:6" ht="39.75" thickBot="1">
-      <c r="A7" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="9">
-        <v>43</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="1:6" ht="27" thickBot="1">
-      <c r="A9" s="7" t="s">
+      <c r="C9" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="9">
-        <v>5</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:6" ht="39.75" thickBot="1">
-      <c r="A12" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" s="9">
-        <v>17</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="39.75" thickBot="1">
-      <c r="A15" s="7"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="39.75" thickBot="1">
-      <c r="A16" s="7"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A17" s="7"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-    </row>
-    <row r="19" spans="1:6" ht="27" thickBot="1">
-      <c r="A19" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19" s="9">
-        <v>32</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="39.75" thickBot="1">
-      <c r="A20" s="7"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A21" s="7"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="27" thickBot="1">
-      <c r="A22" s="7"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A23" s="11"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-    </row>
-    <row r="24" spans="1:6" ht="27" thickBot="1">
-      <c r="A24" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B24" s="9">
-        <v>26</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A25" s="11"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-    </row>
-    <row r="26" spans="1:6" ht="39.75" thickBot="1">
-      <c r="A26" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B26" s="9">
-        <v>12</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A27" s="7"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A28" s="7"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="39.75" thickBot="1">
-      <c r="A29" s="7"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="27" thickBot="1">
-      <c r="A30" s="7"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A31" s="7"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A32" s="7"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="27" thickBot="1">
-      <c r="A33" s="7"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A34" s="11"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-    </row>
-    <row r="35" spans="1:6" ht="27" thickBot="1">
-      <c r="A35" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B35" s="9">
-        <v>37</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A36" s="7"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="27" thickBot="1">
-      <c r="A37" s="7"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:F2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="171" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="39.75" thickBot="1">
+    <row r="1" spans="1:4" ht="16" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="27" thickBot="1">
+    <row r="2" spans="1:4" ht="16" thickBot="1">
       <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
@@ -2023,7 +1575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="27" thickBot="1">
+    <row r="3" spans="1:4" ht="16" thickBot="1">
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
@@ -2037,7 +1589,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="27" thickBot="1">
+    <row r="4" spans="1:4" ht="16" thickBot="1">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -2051,7 +1603,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1">
+    <row r="5" spans="1:4" ht="16" thickBot="1">
       <c r="A5" s="7" t="s">
         <v>28</v>
       </c>
@@ -2063,7 +1615,7 @@
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1">
+    <row r="6" spans="1:4" ht="16" thickBot="1">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>

</xml_diff>